<commit_message>
v4.3: app completo + logo oficial + seeds XLSX
</commit_message>
<xml_diff>
--- a/assets/seed_abastecimentos.xlsx
+++ b/assets/seed_abastecimentos.xlsx
@@ -533,7 +533,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Demo seed 1</t>
+          <t>Demo 1</t>
         </is>
       </c>
     </row>
@@ -565,11 +565,11 @@
         <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>4000</v>
+        <v>0.3</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>m2</t>
+          <t>ha</t>
         </is>
       </c>
       <c r="I3" t="n">
@@ -580,7 +580,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Demo seed 2</t>
+          <t>Demo 2</t>
         </is>
       </c>
     </row>

</xml_diff>